<commit_message>
Cambios - RFC12 NU
</commit_message>
<xml_diff>
--- a/Proyectos/Iteración #4/docs/Extras/Modelo_Relacional.xlsx
+++ b/Proyectos/Iteración #4/docs/Extras/Modelo_Relacional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/c_munoza_uniandes_edu_co/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Working\Working\Git Repositories\C-09\Proyectos\Iteración #4\docs\Extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15D523EE-6A3B-46A3-8E01-8C63EE62CE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A69C7B2-127E-4D66-B7B3-FA3966DF8C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Relación" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="124">
   <si>
     <t>Relación</t>
   </si>
@@ -480,12 +480,21 @@
   <si>
     <t>CK (&gt;=0)</t>
   </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>numOcupamiento</t>
+  </si>
+  <si>
+    <t>duenioAlojamiento</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -999,11 +1008,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="25.7109375" style="2"/>
     <col min="3" max="3" width="44.85546875" style="2" customWidth="1"/>
@@ -1016,7 +1025,7 @@
     <col min="11" max="16384" width="25.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" customHeight="1">
+    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="30" customHeight="1" thickBot="1">
+    <row r="3" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1045,7 +1054,7 @@
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="2:10" s="5" customFormat="1" ht="30" customHeight="1">
+    <row r="4" spans="2:10" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1060,7 +1069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30" customHeight="1">
+    <row r="5" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
@@ -1075,7 +1084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="30" customHeight="1">
+    <row r="6" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I6" s="16" t="s">
         <v>14</v>
       </c>
@@ -1083,7 +1092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="55.15" customHeight="1">
+    <row r="7" spans="2:10" ht="55.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1094,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="40.9" customHeight="1">
+    <row r="8" spans="2:10" ht="40.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1117,7 +1126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="37.15" customHeight="1">
+    <row r="9" spans="2:10" ht="37.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1140,7 +1149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="31.9" customHeight="1">
+    <row r="10" spans="2:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -1153,12 +1162,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="30" customHeight="1">
+    <row r="12" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1">
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1">
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="30" customHeight="1">
+    <row r="15" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1206,12 +1215,12 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1">
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" customHeight="1">
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="30" customHeight="1">
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
@@ -1239,23 +1248,23 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="30" customHeight="1">
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1">
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="30" customHeight="1">
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="30" customHeight="1">
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1275,7 +1284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="30" customHeight="1">
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
@@ -1295,7 +1304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="30" customHeight="1">
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1303,12 +1312,12 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="27" spans="2:8" ht="30" customHeight="1">
+    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="30" customHeight="1">
+    <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>19</v>
       </c>
@@ -1327,9 +1336,11 @@
       <c r="G28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="2:8" ht="30" customHeight="1">
+      <c r="H28" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>26</v>
       </c>
@@ -1348,21 +1359,25 @@
       <c r="G29" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" ht="30" customHeight="1">
+      <c r="H29" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-    </row>
-    <row r="32" spans="2:8" ht="30" customHeight="1">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="30" customHeight="1">
+    <row r="33" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
@@ -1390,8 +1405,11 @@
       <c r="J33" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="2:13" ht="30" customHeight="1">
+      <c r="K33" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>69</v>
       </c>
@@ -1419,8 +1437,11 @@
       <c r="J34" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" ht="30" customHeight="1">
+      <c r="K34" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="7"/>
@@ -1430,13 +1451,14 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-    </row>
-    <row r="37" spans="2:13" ht="30" customHeight="1">
+      <c r="K35" s="6"/>
+    </row>
+    <row r="37" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="2:13" ht="30" customHeight="1">
+    <row r="38" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1455,8 +1477,11 @@
       <c r="G38" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="2:13" ht="30" customHeight="1">
+      <c r="H38" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>69</v>
       </c>
@@ -1475,16 +1500,20 @@
       <c r="G39" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="2:13" ht="30" customHeight="1">
+      <c r="H39" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-    </row>
-    <row r="42" spans="2:13" ht="30" customHeight="1">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="42" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>81</v>
       </c>
@@ -1500,7 +1529,7 @@
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="2:13" ht="30" customHeight="1">
+    <row r="43" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>82</v>
       </c>
@@ -1520,7 +1549,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="2:13" ht="30" customHeight="1">
+    <row r="44" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4" t="s">
         <v>26</v>
       </c>
@@ -1540,7 +1569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="2:13" ht="30" customHeight="1">
+    <row r="45" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -1553,7 +1582,7 @@
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
     </row>
-    <row r="47" spans="2:13" ht="30" customHeight="1">
+    <row r="47" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>87</v>
       </c>
@@ -1562,7 +1591,7 @@
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="2:13" ht="30" customHeight="1">
+    <row r="48" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
         <v>62</v>
       </c>
@@ -1576,7 +1605,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="30" customHeight="1">
+    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="11" t="s">
         <v>91</v>
       </c>
@@ -1591,13 +1620,13 @@
       </c>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="2:8" ht="30" customHeight="1">
+    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="52" spans="2:8" ht="30" customHeight="1">
+    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>94</v>
       </c>
@@ -1605,7 +1634,7 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="2:8" ht="30" customHeight="1">
+    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
         <v>82</v>
       </c>
@@ -1628,7 +1657,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="30" customHeight="1">
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="4" t="s">
         <v>26</v>
       </c>
@@ -1651,7 +1680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="30" customHeight="1">
+    <row r="55" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="7"/>
@@ -1660,7 +1689,7 @@
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="57" spans="2:8" ht="30" customHeight="1">
+    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>100</v>
       </c>
@@ -1669,7 +1698,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
     </row>
-    <row r="58" spans="2:8" ht="30" customHeight="1">
+    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
         <v>62</v>
       </c>
@@ -1683,7 +1712,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="51" customHeight="1">
+    <row r="59" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="11" t="s">
         <v>91</v>
       </c>
@@ -1697,13 +1726,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="30" customHeight="1">
+    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="62" spans="2:8" ht="30" customHeight="1">
+    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>105</v>
       </c>
@@ -1714,7 +1743,7 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="2:8" ht="30" customHeight="1">
+    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
         <v>82</v>
       </c>
@@ -1731,7 +1760,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="30" customHeight="1">
+    <row r="64" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="4" t="s">
         <v>26</v>
       </c>
@@ -1748,21 +1777,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="30" customHeight="1">
+    <row r="65" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
     </row>
-    <row r="67" spans="2:6" ht="30" customHeight="1">
+    <row r="67" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="2:6" ht="30" customHeight="1">
+    <row r="68" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
         <v>62</v>
       </c>
@@ -1773,7 +1802,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="30" customHeight="1">
+    <row r="69" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="11" t="s">
         <v>91</v>
       </c>
@@ -1784,19 +1813,19 @@
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="30" customHeight="1">
+    <row r="70" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="73" spans="2:6" ht="30" customHeight="1">
+    <row r="73" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="2:6" ht="30" customHeight="1">
+    <row r="74" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
         <v>62</v>
       </c>
@@ -1804,7 +1833,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="30" customHeight="1">
+    <row r="75" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="11" t="s">
         <v>115</v>
       </c>
@@ -1812,19 +1841,19 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="30" customHeight="1">
+    <row r="76" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
     </row>
-    <row r="77" spans="2:6" ht="84.6" customHeight="1"/>
-    <row r="78" spans="2:6" ht="30" customHeight="1">
+    <row r="77" spans="2:6" ht="84.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="2:6" ht="30" customHeight="1">
+    <row r="79" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
         <v>34</v>
       </c>
@@ -1835,7 +1864,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="30" customHeight="1">
+    <row r="80" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="11" t="s">
         <v>91</v>
       </c>
@@ -1846,7 +1875,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="2:4" ht="30" customHeight="1">
+    <row r="81" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>

</xml_diff>